<commit_message>
Update Zdetl Correlative Words.xlsx
</commit_message>
<xml_diff>
--- a/Zdetl Correlative Words.xlsx
+++ b/Zdetl Correlative Words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkaz1\Documents\GitHub\Zdetl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{392D80C7-7A27-44AE-A03F-0D612BE2446B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE404506-2985-4D7A-8037-A1FB0C0E2CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30945" yWindow="2085" windowWidth="18045" windowHeight="10035" xr2:uid="{8D6C5578-70E6-4DFE-83FE-5AE0AAF0D81A}"/>
+    <workbookView xWindow="30510" yWindow="1650" windowWidth="17280" windowHeight="8970" xr2:uid="{8D6C5578-70E6-4DFE-83FE-5AE0AAF0D81A}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlative Words" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Zdetl Correlative Words</t>
   </si>
@@ -214,6 +214,36 @@
   </si>
   <si>
     <t>Kind or Type (-ochti)</t>
+  </si>
+  <si>
+    <t>Any (zi-)</t>
+  </si>
+  <si>
+    <t>zi-tetl</t>
+  </si>
+  <si>
+    <t>zi-ad</t>
+  </si>
+  <si>
+    <t>zi-zhia</t>
+  </si>
+  <si>
+    <t>zi-qez</t>
+  </si>
+  <si>
+    <t>zi-patle</t>
+  </si>
+  <si>
+    <t>zi-qenta</t>
+  </si>
+  <si>
+    <t>zi-qik</t>
+  </si>
+  <si>
+    <t>zi-adl</t>
+  </si>
+  <si>
+    <t>zi-ochti</t>
   </si>
 </sst>
 </file>
@@ -281,13 +311,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2F02EF-6620-4665-9DA6-9AA40A77A4C6}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,217 +650,248 @@
     <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="G4" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="G5" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="G6" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="G7" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="G8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="G9" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="G10" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>